<commit_message>
Update document test, création manuel d'installation et utilisation ainsi que glossaire
Tous des documents séparés qui seront réuni à la fin du pré-tpi
</commit_message>
<xml_diff>
--- a/1. Pré-TPI/Rendu/7. Stratégie de test.xlsx
+++ b/1. Pré-TPI/Rendu/7. Stratégie de test.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t>Type de test</t>
   </si>
@@ -121,13 +121,46 @@
     <t>ý</t>
   </si>
   <si>
-    <t>Test du fichier test</t>
-  </si>
-  <si>
-    <t>que l'entier de la ligne soit remplie correctement</t>
-  </si>
-  <si>
-    <t>Siiiiiiiiiii</t>
+    <t>Nom du test</t>
+  </si>
+  <si>
+    <t>But du test</t>
+  </si>
+  <si>
+    <t>Machines concernées</t>
+  </si>
+  <si>
+    <t>Problème possible</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>¨</t>
+  </si>
+  <si>
+    <t>Date du test</t>
+  </si>
+  <si>
+    <t>Test fonctionnement Fortigate 80F</t>
+  </si>
+  <si>
+    <t>Vérifier que l'appareil fonctionne</t>
+  </si>
+  <si>
+    <t>FortiGate 80F + PC05</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Brancher le FortiG 80F selon manuel d'installation</t>
+  </si>
+  <si>
+    <t>Accès au login du FG 80F</t>
+  </si>
+  <si>
+    <t>Connexion réussite</t>
   </si>
 </sst>
 </file>
@@ -219,10 +252,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -235,6 +267,13 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,199 +555,239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
+      </c>
+      <c r="C2" s="9">
+        <v>44985</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F3" s="9"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F10" s="9"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F11" s="9"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="9"/>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="9"/>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="9"/>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="9"/>
-    </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="9"/>
-    </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F23" s="9"/>
-    </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F24" s="9"/>
-    </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F25" s="9"/>
-    </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F26" s="9"/>
-    </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F28" s="9"/>
-    </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F29" s="9"/>
-    </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F31" s="9"/>
-    </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F32" s="9"/>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F34" s="9"/>
-    </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F35" s="9"/>
-    </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F36" s="9"/>
-    </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F37" s="9"/>
-    </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F38" s="9"/>
-    </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F39" s="9"/>
-    </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F40" s="9"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="8"/>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I26" s="8"/>
+    </row>
+    <row r="27" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I28" s="8"/>
+    </row>
+    <row r="29" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I29" s="8"/>
+    </row>
+    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I30" s="8"/>
+    </row>
+    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I31" s="8"/>
+    </row>
+    <row r="32" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I32" s="8"/>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I33" s="8"/>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I34" s="8"/>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="8"/>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I36" s="8"/>
+    </row>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I37" s="8"/>
+    </row>
+    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I38" s="8"/>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I39" s="8"/>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I40" s="8"/>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I41" s="8"/>
+    </row>
+    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I42" s="8"/>
+    </row>
+    <row r="43" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I43" s="8"/>
+    </row>
+    <row r="44" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I44" s="8"/>
+    </row>
+    <row r="45" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I45" s="8"/>
+    </row>
+    <row r="46" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I46" s="8"/>
+    </row>
+    <row r="47" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I47" s="8"/>
+    </row>
+    <row r="48" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I48" s="8"/>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I49" s="8"/>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I50" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Paramètres!$A$2:$A$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2:A40</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Paramètres!$B$2:$B$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B40</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Paramètres!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F40</xm:sqref>
+          <xm:sqref>I2:I50</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -726,7 +805,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53" style="1" bestFit="1" customWidth="1"/>
@@ -736,16 +815,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -761,19 +840,19 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -795,22 +874,22 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -825,7 +904,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:F16"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,14 +913,14 @@
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -852,7 +931,7 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -863,7 +942,7 @@
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -873,6 +952,9 @@
       </c>
       <c r="B4" t="s">
         <v>11</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>